<commit_message>
updated thermal curve data
</commit_message>
<xml_diff>
--- a/data/oxygen-correlation/resazurin_metadata.xlsx
+++ b/data/oxygen-correlation/resazurin_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/resazurin-assay-development/data/oxygen-correlation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EC077F-4EFF-8E47-9065-638DBD460DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFC1044-3C16-134F-A6CD-4614049DA9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6960" yWindow="760" windowWidth="19460" windowHeight="17760" xr2:uid="{F9B76D48-E646-9D48-9AB8-3319F507EDF2}"/>
   </bookViews>
@@ -885,7 +885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7159BF13-8618-0540-AFAB-AF0D60C37565}">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>

</xml_diff>